<commit_message>
codes pour nettoyer données datagouv et données datagouv_affiliations + code pour extraction liste cote_etab
</commit_message>
<xml_diff>
--- a/data/codes_etab.xlsx
+++ b/data/codes_etab.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B154"/>
+  <dimension ref="A1:C234"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -368,6 +368,11 @@
           <t>universites</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>anciens_noms</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -380,11 +385,17 @@
           <t>Antilles-Guyane</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Voir ANTI à partir de 2015-06-25_x000D_
+		Voir YANE à partir de 2015-03-16</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">AIXM </t>
+          <t>AIXM</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -404,6 +415,11 @@
           <t>Aix-Marseille 1</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Voir AIXM à  partir de 2012-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -416,6 +432,11 @@
           <t>Aix-Marseille 2</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Voir AIXM à  partir de 2012-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -428,11 +449,16 @@
           <t>Aix-Marseille 3</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Voir AIXM à  partir de 2012-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">ALGF </t>
+          <t>ALGF</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -444,7 +470,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">AMIE </t>
+          <t>AMIE</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -456,7 +482,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">ANGE </t>
+          <t>ANGE</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -468,7 +494,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">ANTI </t>
+          <t>ANTI</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -480,7 +506,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">ARTO </t>
+          <t>ARTO</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -492,7 +518,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">ASSA </t>
+          <t>ASSA</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -504,7 +530,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">AVIG </t>
+          <t>AVIG</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -524,6 +550,11 @@
           <t>Université Côte d'Azur (ComUE)</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Voir COAZ à  partir de 2020-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -536,6 +567,11 @@
           <t>Belfort Montbéliard</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Voir UBFC de 2017-01-01 à 2024-12-31</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -548,11 +584,17 @@
           <t>Besançon</t>
         </is>
       </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Voir UBFC de 2017-01-01 à 2024-12-31 _x000D_
+    puis PAST à partir de 2025-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">BORD </t>
+          <t>BORD</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -572,6 +614,11 @@
           <t>Université de Bordeaux (1441-1970)</t>
         </is>
       </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Voir BOR1, BOR2 ou BOR3 à  partir de 1970-11-13</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -584,6 +631,12 @@
           <t>Bordeaux 1</t>
         </is>
       </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Voir BOR4 à  partir de 1995-05-09 (pour les thèses de Droit, Sciences sociales et politiques, Sciences économiques et Gestion)_x000D_
+    Voir BORD à  partir de 2014-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -596,11 +649,16 @@
           <t>Bordeaux 2</t>
         </is>
       </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Voir BORD à  partir de 2014-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve">BOR3 </t>
+          <t>BOR3</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -617,14 +675,19 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Bordeaux 4</t>
+          <t>Bordeaux 4</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Voir BORD à  partir de 2014-01-01</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t xml:space="preserve">BRES </t>
+          <t>BRES</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -644,6 +707,11 @@
           <t>Caen</t>
         </is>
       </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Voir NORM à  partir de 2017-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -656,6 +724,11 @@
           <t>Cergy-Pontoise</t>
         </is>
       </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Voir CYUN à  partir de 2020-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -668,6 +741,12 @@
           <t>Chambéry</t>
         </is>
       </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Voir GREN de 2010-11-01 à  2014-12-31_x000D_
+	Voir GREA de 2015-01-01 à  2019-12-31</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -680,6 +759,11 @@
           <t>Université de Clermont-Ferrand</t>
         </is>
       </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Voir CFL1 ou CFL2 à  partir de 1976-03-16</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -692,6 +776,11 @@
           <t>Université Clermont Auvergne (2017-2020)</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Voir UCFA à  partir de 2021-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -704,6 +793,11 @@
           <t>Clermont-Ferrand 1</t>
         </is>
       </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Voir CLFA à  partir de 2017-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -716,11 +810,16 @@
           <t>Clermont-Ferrand 2</t>
         </is>
       </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Voir CLFA à  partir de 2017-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t xml:space="preserve">COAZ </t>
+          <t>COAZ</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -732,7 +831,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t xml:space="preserve">COMP </t>
+          <t>COMP</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -744,7 +843,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t xml:space="preserve">CORT </t>
+          <t>CORT</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -756,7 +855,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t xml:space="preserve">CYUN </t>
+          <t>CYUN</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -776,11 +875,17 @@
           <t>Dijon</t>
         </is>
       </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Voir UBFC de 2017-01-01 à 2024-12-31_x000D_
+        puis UBEU à partir de 2025-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t xml:space="preserve">DUNK </t>
+          <t>DUNK</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -800,11 +905,17 @@
           <t>Evry Val d'Essonne</t>
         </is>
       </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Voir SACL de 2015-09-01 à 2019-12-31_x000D_
+	Voir UPAS à  partir de 2020-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t xml:space="preserve">GRAL </t>
+          <t>GRAL</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -824,6 +935,11 @@
           <t>Université Grenoble Alpes (ComUE)</t>
         </is>
       </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Voir GRAL à  partir de 2020-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -836,6 +952,11 @@
           <t>Grenoble</t>
         </is>
       </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Voir GREA à  partir de 2015-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -848,6 +969,11 @@
           <t>Grenoble 1</t>
         </is>
       </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Voir GREN à  partir de 2010-11-01</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -860,6 +986,11 @@
           <t>Grenoble 2</t>
         </is>
       </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Voir GREN à  partir de 2010-11-01</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -872,6 +1003,11 @@
           <t>Grenoble 3</t>
         </is>
       </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Voir GREN à  partir de 2010-11-01</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -884,6 +1020,11 @@
           <t>Faculté de Droit et Sciences économiques de Grenoble</t>
         </is>
       </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Voir GRE2 à  partir de 1970-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -896,6 +1037,11 @@
           <t>Faculté de Lettres et Sciences humaines de Grenoble</t>
         </is>
       </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Voir GRE3 à  partir de 1970-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -908,6 +1054,11 @@
           <t>Faculté de droit de Grenoble</t>
         </is>
       </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Voir GFDE à  partir de 1896-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -920,11 +1071,16 @@
           <t>Faculté de Lettres de Grenoble</t>
         </is>
       </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Voir GFLH à  partir de 1896-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t xml:space="preserve">LARE </t>
+          <t>LARE</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -936,7 +1092,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t xml:space="preserve">LARO </t>
+          <t>LARO</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -956,11 +1112,16 @@
           <t>Le Havre</t>
         </is>
       </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Voir NORM à  partir de 2017-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t xml:space="preserve">LEMA </t>
+          <t>LEMA</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -980,6 +1141,11 @@
           <t>Université de Lille (2018-2021)</t>
         </is>
       </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Voir ULIL à partir de 2022-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -992,6 +1158,11 @@
           <t>Lille 1</t>
         </is>
       </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Voir LILU à  partir de 2018-01-15</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1004,6 +1175,11 @@
           <t>Lille 2</t>
         </is>
       </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Voir LILU à  partir de 2018-01-15</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1016,6 +1192,11 @@
           <t>Lille 3</t>
         </is>
       </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Voir LILU à  partir de 2018-01-15</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1028,6 +1209,11 @@
           <t>Faculté des sciences de Lille</t>
         </is>
       </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Voir LILL à  partir de 1896-07-10</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1040,11 +1226,18 @@
           <t>Université de Lille (1896-1970)</t>
         </is>
       </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Voir LIL1 à  partir de 1969-12-18_x000D_
+    Voir LIL2 à  partir de 1971-01-01_x000D_
+    Voir LIL3 à  partir de 1969-12-18</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t xml:space="preserve">LIMO </t>
+          <t>LIMO</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1056,7 +1249,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t xml:space="preserve">LORI </t>
+          <t>LORI</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1068,7 +1261,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t xml:space="preserve">LORR </t>
+          <t>LORR</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1088,6 +1281,11 @@
           <t>Lyon 1</t>
         </is>
       </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Voir LYSE de 2015-03-01 à 2022-08-31</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1100,6 +1298,11 @@
           <t>Lyon 2</t>
         </is>
       </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Voir LYSE de 2015-03-01 à 2022-08-31</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1112,6 +1315,11 @@
           <t>Lyon 3</t>
         </is>
       </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Voir LYSE de 2015-03-01 à 2022-08-31</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1124,6 +1332,11 @@
           <t>Faculté de médecine et de pharmacie de Lyon</t>
         </is>
       </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Voir LYON à  partir de 1896-07-10</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1136,6 +1349,11 @@
           <t>Faculté de sciences de Lyon</t>
         </is>
       </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Voir LYON à  partir de 1896-07-10</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1148,6 +1366,11 @@
           <t>Ecole préparatoire de médecine et de pharmacie de Lyon</t>
         </is>
       </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Voir LYFM à  partir de 1874-11-08</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1160,6 +1383,13 @@
           <t>Université de Lyon</t>
         </is>
       </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Voir LYO1 à  partir de 1969-12-05_x000D_
+    Voir LYO2 à  partir de 1969-12-05_x000D_
+    Voir LYO3 à  partir de 1973-07-26</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1172,6 +1402,11 @@
           <t>Lyon (COMUE)</t>
         </is>
       </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Voir LYO1, LYO2, LYO3, ECDL, ENSL, ENTP, ESAL, STET, VETA à partir de 2022-08-31</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1184,6 +1419,11 @@
           <t>Marne la Vallée</t>
         </is>
       </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Voir PEST à  partir de 2008-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1196,6 +1436,11 @@
           <t>Metz</t>
         </is>
       </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Voir LORR à  partir de 2012-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1208,6 +1453,11 @@
           <t>Montpellier</t>
         </is>
       </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Voir UMON à partir de 2022-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1220,6 +1470,11 @@
           <t>Montpellier 1</t>
         </is>
       </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Voir MONT à  partir de 2015-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1232,6 +1487,11 @@
           <t>Montpellier 2</t>
         </is>
       </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Voir MONT à  partir de 2015-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1244,11 +1504,16 @@
           <t>Montpellier 3</t>
         </is>
       </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Voir UMPV à partir de 2025-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t xml:space="preserve">MULH </t>
+          <t>MULH</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1268,6 +1533,11 @@
           <t>Faculté de droit de Nancy</t>
         </is>
       </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Voir NAN2 à  partir de 1970-12-23</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1280,6 +1550,11 @@
           <t>Faculté des lettres de Nancy</t>
         </is>
       </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Voir NAN2 à  partir de 1970-12-23</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1292,6 +1567,11 @@
           <t>Faculté des sciences de Nancy</t>
         </is>
       </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Voir NAN1 à  partir de 1970-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1304,6 +1584,11 @@
           <t>Nancy 1</t>
         </is>
       </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Voir LORR à  partir de 2012-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1316,6 +1601,11 @@
           <t>Nancy 2</t>
         </is>
       </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Voir LORR à  partir de 2012-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1328,11 +1618,16 @@
           <t>Nantes</t>
         </is>
       </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Voir NANU àpartir de 2022-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t xml:space="preserve">NANU </t>
+          <t>NANU</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -1344,7 +1639,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t xml:space="preserve">NCAL </t>
+          <t>NCAL</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1364,6 +1659,11 @@
           <t>Nice</t>
         </is>
       </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Voir AZUR à  partir de 2016-09-01</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1376,11 +1676,16 @@
           <t>Nîmes</t>
         </is>
       </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Voir NIMU à partir de 2025-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t xml:space="preserve">NIMU </t>
+          <t>NIMU</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1392,7 +1697,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t xml:space="preserve">NORM </t>
+          <t>NORM</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1404,7 +1709,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t xml:space="preserve">ORLE </t>
+          <t>ORLE</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1424,11 +1729,17 @@
           <t>Université de Paris (1896-1968)</t>
         </is>
       </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Voir PA01, PA02, PA03, PA04, PA05, PA06, PA07, PA08, PA09, PA10, PA11, PA12, PA13 à  partir de 1970-03-21_x000D_
+    ATTENTION : la date officielle de fin est 1968 mais ce libellé couvre les thèses soutenues jusqu'au 1970-12-31 date à  laquelle l'université de Paris créée en 1896 a définitivement cessé d'exister</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t xml:space="preserve">PA01 </t>
+          <t>PA01</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -1448,6 +1759,11 @@
           <t>Paris 2</t>
         </is>
       </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Voir ASSA à partir de 2022-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1460,6 +1776,11 @@
           <t>Paris 3</t>
         </is>
       </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Voir USPC de 2015-01-01 à  2019-08-31</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -1472,6 +1793,11 @@
           <t>Paris 4</t>
         </is>
       </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Voir SORU à  partir de 2018-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -1484,6 +1810,12 @@
           <t>Paris 5</t>
         </is>
       </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Voir USPC de 2015-01-01 à  2019-08-31_x000D_
+        Voir UNIP à  partir de 2019-09-01</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1496,6 +1828,11 @@
           <t>Paris 6</t>
         </is>
       </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Voir SORU à  partir de 2018-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -1508,11 +1845,17 @@
           <t>Paris 7</t>
         </is>
       </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Voir USPC de 2015-01-01 à  2019-08-31_x000D_
+        Voir UNIP à  partir de 2019-09-01</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t xml:space="preserve">PA08 </t>
+          <t>PA08</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -1532,11 +1875,17 @@
           <t>Paris 9</t>
         </is>
       </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Voir PSLE de 2016-01-01 à  2019-12-31_x000D_
+	Voir UPSL à  partir de 2020-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t xml:space="preserve">PA10 </t>
+          <t>PA10</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -1556,6 +1905,12 @@
           <t>Paris 11</t>
         </is>
       </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Voir SACL de 2015-09-01 à  2019-12-31_x000D_
+	Voir UPAS à  partir de 2020-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -1568,6 +1923,11 @@
           <t>Paris 12</t>
         </is>
       </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Voir PEST de 2008-01-01 à 2020-09-01</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -1580,6 +1940,11 @@
           <t>Paris 13</t>
         </is>
       </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>(Voir USPC de 2015-01-01 à  2019-08-31)</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -1592,6 +1957,12 @@
           <t>Pacifique</t>
         </is>
       </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Voir NCAL à  partir de 1999-06-01_x000D_
+		Voir POLF à  partir de 1999-06-01</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -1604,6 +1975,11 @@
           <t>Faculté de Droit de Paris</t>
         </is>
       </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Voir PA00 à  partir de 1896-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -1616,6 +1992,11 @@
           <t>Faculté des Lettres de Paris</t>
         </is>
       </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Voir PA00 à  partir de 1896-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -1628,6 +2009,11 @@
           <t>Faculté de Médecine de Paris</t>
         </is>
       </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Voir PA00 à  partir de 1896-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -1640,6 +2026,11 @@
           <t>Faculté des Sciences de Paris</t>
         </is>
       </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Voir PA00 à  partir de 1896-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -1652,11 +2043,16 @@
           <t>Ecole supérieure de pharmacie de Paris</t>
         </is>
       </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Voir PA00 à  partir de 1920-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t xml:space="preserve">PAST </t>
+          <t>PAST</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -1676,6 +2072,11 @@
           <t>Faculté de Théologie catholique de Paris</t>
         </is>
       </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Voir PA00 à  partir de 1885-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -1688,11 +2089,16 @@
           <t>Faculté de Théologie protestante de Paris</t>
         </is>
       </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Voir PA00 de 1896-01-01 à  1905-01-0</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t xml:space="preserve">PAUU </t>
+          <t>PAUU</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -1704,7 +2110,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t xml:space="preserve">PERP </t>
+          <t>PERP</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -1716,7 +2122,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t xml:space="preserve">PESC </t>
+          <t>PESC</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -1736,11 +2142,16 @@
           <t>Paris Est (PRES)</t>
         </is>
       </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Voir PESC à  partir de 2015-03-01</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t xml:space="preserve">POIT </t>
+          <t>POIT</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -1752,7 +2163,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t xml:space="preserve">POLF </t>
+          <t>POLF</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -1764,7 +2175,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t xml:space="preserve">REIM </t>
+          <t>REIM</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -1784,6 +2195,11 @@
           <t>Université de Rennes</t>
         </is>
       </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Voir REN1 ou REN2 à  partir de 1971-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -1796,11 +2212,16 @@
           <t>Rennes 1</t>
         </is>
       </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Voir UREN à partir de 2023-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t xml:space="preserve">REN2 </t>
+          <t>REN2</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -1820,6 +2241,11 @@
           <t>Rouen</t>
         </is>
       </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Voir NORM à  partir de 2017-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -1832,11 +2258,16 @@
           <t>Université Paris-Saclay (ComUE)</t>
         </is>
       </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Voir UPAS à  partir de 2020-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t xml:space="preserve">SORU </t>
+          <t>SORU</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -1856,11 +2287,17 @@
           <t>Saint-Etienne</t>
         </is>
       </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Voir LYSE de 2015-03-01 à 2022-08-31_x000D_
+      Voir UJMO à partir du 2025-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t xml:space="preserve">STRA </t>
+          <t>STRA</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -1880,6 +2317,11 @@
           <t>Strasbourg 1</t>
         </is>
       </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Voir STRA à  partir de 2009-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -1892,6 +2334,11 @@
           <t>Strasbourg 2</t>
         </is>
       </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Voir STRA à  partir de 2009-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -1904,11 +2351,16 @@
           <t>Strasbourg 3</t>
         </is>
       </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Voir STRA à  partir de 2009-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t xml:space="preserve">TLSE </t>
+          <t>TLSE</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -1928,6 +2380,11 @@
           <t>Toulouse 1</t>
         </is>
       </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Voir TOUC à partir de 2023-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -1940,6 +2397,11 @@
           <t>Toulouse 2</t>
         </is>
       </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Voir TLSE à partir de 2024-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -1952,11 +2414,16 @@
           <t>Toulouse 3</t>
         </is>
       </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Voir TLSE à partir de 2024-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t xml:space="preserve">TOUC </t>
+          <t>TOUC</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -1968,7 +2435,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t xml:space="preserve">TOUL </t>
+          <t>TOUL</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -1980,7 +2447,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t xml:space="preserve">TOUR </t>
+          <t>TOUR</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -1992,7 +2459,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t xml:space="preserve">TROY </t>
+          <t>TROY</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -2004,7 +2471,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t xml:space="preserve">UBEU </t>
+          <t>UBEU</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -2024,11 +2491,16 @@
           <t>Bourgogne Franche-Comté</t>
         </is>
       </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Voir PAST, UBEU, SUPM, BELF, AGRO à partir de 2025-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t xml:space="preserve">UCFA </t>
+          <t>UCFA</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -2040,7 +2512,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t xml:space="preserve">UEFL </t>
+          <t>UEFL</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -2052,7 +2524,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t xml:space="preserve">UJMO </t>
+          <t>UJMO</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -2064,7 +2536,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t xml:space="preserve">ULIL </t>
+          <t>ULIL</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -2076,7 +2548,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t xml:space="preserve">UMPV </t>
+          <t>UMPV</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -2088,7 +2560,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t xml:space="preserve">UMON </t>
+          <t>UMON</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -2100,7 +2572,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t xml:space="preserve">UNIP </t>
+          <t>UNIP</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -2112,7 +2584,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t xml:space="preserve">UPAS </t>
+          <t>UPAS</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -2124,7 +2596,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t xml:space="preserve">UPHF </t>
+          <t>UPHF</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -2136,7 +2608,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t xml:space="preserve">UPSL </t>
+          <t>UPSL</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -2148,7 +2620,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t xml:space="preserve">UREN </t>
+          <t>UREN</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -2168,6 +2640,11 @@
           <t>Sorbonne Paris Cité</t>
         </is>
       </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Voir PA03, PA13, INAL et UNIP à  partir de 2019-09-01</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -2180,6 +2657,11 @@
           <t>Valenciennes</t>
         </is>
       </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Voir UPHF à partir de 2019-09-09</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -2192,16 +2674,1230 @@
           <t>Versailles St Quentin en Yvelines</t>
         </is>
       </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Voir SACL de 2015-09-01 à  2019-12-31_x000D_
+	Voir UPAS à  partir de 2020-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t xml:space="preserve">YANE </t>
+          <t>YANE</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
           <t>Guyane</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>INPG</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Institut national polytechnique - Grenoble</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Voir GREN à  partir de 2010-11-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>INPL</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Institut national polytechnique - Lorraine</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>INPT</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Institut national polytechnique - Toulouse</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Voir TLSE à partir de 2024-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>IPPA</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Institut Polytechnique de Paris</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>AGRO</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Institut Agro</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>AGPT</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>AgroParisTech</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Voir aussi SACL de 2015-09-01 à  2019-12-31_x000D_
+    Voir aussi UPAS à  partir de 2020-01-01_x000D_
+	Voir aussi IAVF à  partir de 2016-09-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>CLIL</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Centrale Lille Institut</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>CNAM</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Conservatoire national des arts et métiers</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>CSUP</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>CentraleSupélec</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Voir aussi SACL de 2015-09-01 à  2019-12-31_x000D_
+	Voir aussi UPAS à  partir de 2020-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>DENS</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Ecole normale supérieure - Cachan</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Voir SACL de 2015-09-01 à  2019-12-31_x000D_
+	Voir UPAS à  partir de 2020-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>ECAP</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Ecole centrale des arts et manufactures de Paris</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Voir SACL de 2015-09-01 à  2019-12-31_x000D_
+	Voir UPAS à  partir de 2020-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>ECDL</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Ecole centrale de Lyon</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Voir LYSE de 2015-03-01 à 2022-08-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>ECLI</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Ecole centrale de Lille</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Voir CLIL à partir de 2020-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>ECDM</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Ecole centrale de Marseille</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>EHEC</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Ecole des hautes études commerciales</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Voir SACL de 2015-09-01 à  2019-08-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>EHES</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Ecole des hautes études en sciences sociales</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>EIAA</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Ecole nationale supérieure des industries alimentaires - Massy</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Voir AGPT à  partir de 2007-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>EMAC</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Ecole nationale des Mines d'Albi-Carmaux</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>EMAL</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>IMT Mines Alès</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>EMNA</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Ecole des Mines de Nantes</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Voir IMTA à  partir de 2017-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>EMSE</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Ecole nationale supérieure des Mines - Saint-Etienne</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>ENAM</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Ecole nationale supérieure d'arts et métiers</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Voir HESA de 2020-01-01 à 2024-07-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>ENAC</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Ecole nationale de l'aviation civile</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>ENCM</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Ecole nationale supérieure de chimie de Montpellier</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>ENCP</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Ecole nationale des chartes</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>ENCR</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Ecole nationale supérieure de chimie de Rennes</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Voir UREN à partir de 2023-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>ENGR</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Ecole nationale du génie rural, des eaux et forêts</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Voir AGPT à  partir de 2007-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>ENIB</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Ecole nationale d'ingénieurs de Brest</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>ENIS</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Ecole nationale d'ingénieurs de Saint-Etienne</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Voir LYSE de 2015-03-01 à 2022-08-31_x000D_
+Voir ECDL à partir de 2022-09-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>ENMP</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Ecole nationale supérieure des Mines - Paris</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Voir PSLE de 2016-01-01 à  2019-12-31_x000D_
+	Voir UPSL à  partir de 2020-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>ENPC</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Ecole nationale des ponts et chaussées</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Voir PEST de 2008-01-01 à 2020-09-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>ENSA</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Ecole nationale supérieure d'agronomie - Montpellier</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>Voir NSAM à  partir de 2007-12-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>ENSF</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Ecole normale supérieure lettres et sciences humaines - Lyon  _x000D_
+    (anciennement Ecole normale supérieure lettres et sciences humaines - Fontenay-Saint-Cloud</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>Voir ENSL à  partir de 2009-12-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>ENSL</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Ecole normale supérieure (sciences) - Lyon_x000D_
+    Voir Ecole normale supérieure de Lyon à  partir de 2009-12-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>ENSL</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Ecole normale supérieure de Lyon</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Voir LYSE de 2015-03-01 à 2022-08-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>ENSR</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Ecole normale supérieure de Rennes</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>Voir UREN à partir de 2023-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>ENST</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Ecole nationale supérieure des télécommunications</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>Voir SACL de 2015-09-01 à  2019-08-31_x000D_
+    Voir IPPA à  partir de 2019-09-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>ENSU</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Ecole normale supérieure- Paris (rue d'Ulm)</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>Voir PSLE de 2016-01-01 à  2019-12-31_x000D_
+	Voir UPSL à  partir de 2020-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>ENTA</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Ecole nationale supérieure de techniques avancées Bretagne</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>Voir ESTA à partir de 2025-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>ENTP</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Ecole nationale des travaux publics</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>Voir LYSE de 2015-03-01 à 2022-08-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>ENVA</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Ecole nationale vétérinaire - Maisons Alfort</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>EPHE</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Ecole pratique des hautes études</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>Voir PSLE de 2016-01-01 à  2019-12-31_x000D_
+	Voir UPSL à  partir de 2020-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>EPXX</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Ecole polytechnique</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>Voir SACL de 2015-09-01 à  2019-08-31_x000D_
+    Voir IPPA à  partir de 2019-09-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>ESAE</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>ISAE_x000D_
+    (Fusion de SUPAERO et ENSICA à  partir de 2007-01-01)</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>ESAL</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>École nationale supérieure d'architecture - Lyon</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>ESEC</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Ecole supérieure des sciences économiques et commerciales</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>ESMA</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Ecole nationale supérieure de mécanique et d'aérotechnique</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>ESTA</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Ecole nationale supérieure de techniques avancées</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>Voir SACL de 2015-09-01 à  2019-08-31_x000D_
+    Voir, pour partie, IPPA à  partir de 2019-09-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>GLOB</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Institut de physique du Globe</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>Voir USPC à  partir de 2015-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>HESA</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>HESAM</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>Voir CNAM et ENAM à partir de 2024-08-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>HESP</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Ecole des hautes études en santé publique - Rennes</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>IAVF</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Institut agronomique, vétérinaire et forestier de France - Paris</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>IEPP</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Institut d'études politiques - Paris</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>IMTA</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Ecole nationale supérieure Mines-Télécom Atlantique Bretagne Pays de la Loire</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>INAL</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Institut national des langues et civilisations orientales (INALCO)</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>(Voir USPC de 2015-01-01 à  2019-08-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>INAP</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Institut national d'agronomie - Paris Grignon</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>Voir AGPT à  partir de 2007-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>IOTA</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Institut d'optique théorique et appliquée - Palaiseau</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>Voir SACL de 2015-09-01 à  2019-12-31_x000D_
+	Voir UPAS à  partir de 2020-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>ISAB</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Institut national des sciences appliquées Val de Loire - Bourges</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>ISAL</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Institut national des sciences appliquées - Lyon</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>Voir LYSE de 2015-03-01 à 2022-08-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>ISAM</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Institut national des sciences appliquées - Rouen</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>Voir NORM à  partir de 2017-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>ISAR</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Institut national des sciences appliquées - Rennes</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>ISAT</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Institut national des sciences appliquées - Toulouse</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>Voir TLSE à partir de 2024-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>LY01</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Ecole nationale vétérinaire - Lyon</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>MNHN</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Museum d'histoire naturelle</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>MTLD</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Ecole nationale supérieure Mines-Télécom Lille Douai</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>NANT</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Ecole nationale vétérinaire - Nantes</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>Voir ONIR à  partir de 2008-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>NSAI</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Ecole nationale de la Statistique et de l'Analyse de l'Information - Rennes</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>NSAM</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>SupAgro - Montpellier</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>Voir AGRO à partir de 2020-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>NSAR</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>ENSA - Rennes</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>voir NSAR à  partir de 2004-01-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>NSAR</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Agrocampus - Rennes</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>voir NSAR à  partir de 2008-07-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>NSAR</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Agrocampus Ouest - Rennes</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>Voir AGRO à partir de 2020-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>OBSP</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Observatoire de Paris</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>Voir PSLE de 2016-01-01 à  2019-12-31_x000D_
+	Voir UPSL à  partir de 2020-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>ONIR</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Ecole nationale vétérinaire - Nantes</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>PSLE</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Paris Sciences et Lettres (ComUE)</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>Voir UPSL à  partir de 2020-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>SUPL</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Supélec</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>Voir CSUP à  partir de 2015-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>SUPM</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Besançon, École Nationale Supérieure de Mécanique et des Microtechniques</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>TELB</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Ecole nationale supérieure des Telecom de Bretagne - Brest</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>Voir IMTA à  partir de 2017-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>TELE</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Institut national des télécommunications</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>Voir SACL de 2015-09-01 à  2019-08-31_x000D_
+    Voir IPPA à  partir de 2019-09-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>TOU3</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Ecole nationale vétérinaire - Toulouse</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>VETA</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>VetAgro Sup – Marcy l'Etoile</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
correction fichier codes_etab et codes appariemment probabilistes codes_etab et affiliations
</commit_message>
<xml_diff>
--- a/data/codes_etab.xlsx
+++ b/data/codes_etab.xlsx
@@ -3182,8 +3182,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Ecole normale supérieure lettres et sciences humaines - Lyon  _x000D_
-    (anciennement Ecole normale supérieure lettres et sciences humaines - Fontenay-Saint-Cloud</t>
+          <t xml:space="preserve">Ecole normale supérieure lettres et sciences humaines - Lyon  </t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -3200,8 +3199,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Ecole normale supérieure (sciences) - Lyon_x000D_
-    Voir Ecole normale supérieure de Lyon à  partir de 2009-12-10</t>
+          <t>Ecole normale supérieure (sciences) - Lyon</t>
         </is>
       </c>
     </row>
@@ -3365,8 +3363,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>ISAE_x000D_
-    (Fusion de SUPAERO et ENSICA à  partir de 2007-01-01)</t>
+          <t>ISAE</t>
         </is>
       </c>
     </row>

</xml_diff>